<commit_message>
Correction : Erreur Changement de date
</commit_message>
<xml_diff>
--- a/Artéfacts/Artéfacts Sprint 2/Calendrier Sprint 2.xlsx
+++ b/Artéfacts/Artéfacts Sprint 2/Calendrier Sprint 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donoc\Desktop\L3 Informatique\Semestre 2\Projet de développement\Artéfacts\Artéfacts Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC76C95-FB52-4B10-9FCA-ECA7DF436BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFF8775-1BC3-4489-816B-5CEB19E4445C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9DAF1FEF-636C-495F-A4D9-98A6306D3E56}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t>Tâches / Date</t>
   </si>
   <si>
-    <t>Tâche terminé le 21/02/2024</t>
-  </si>
-  <si>
     <t>Extraction du nom du fichier d’origine</t>
   </si>
   <si>
@@ -144,19 +141,22 @@
     <t>Tâches terminé le 18/02/2024</t>
   </si>
   <si>
-    <t>Tâches terminé le 24/02/2024</t>
-  </si>
-  <si>
-    <t>Tâches terminé le 25/02/2024</t>
-  </si>
-  <si>
-    <t>Tâche terminé le 26/02/2024</t>
-  </si>
-  <si>
-    <t>Tâche terminé le 28/02/2024</t>
-  </si>
-  <si>
-    <t>Tâches terminé le 01/03/2024</t>
+    <t>Tâches terminé le 06/02/2024</t>
+  </si>
+  <si>
+    <t>Tâche terminé le 09/02/2024</t>
+  </si>
+  <si>
+    <t>Tâches terminé le 12/02/2024</t>
+  </si>
+  <si>
+    <t>Tâches terminé le 13/02/2024</t>
+  </si>
+  <si>
+    <t>Tâche terminé le 14/02/2024</t>
+  </si>
+  <si>
+    <t>Tâche terminé le 16/02/2024</t>
   </si>
 </sst>
 </file>
@@ -267,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -284,7 +284,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
@@ -602,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25C790B-9A69-420E-ADEC-218324962F86}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,60 +662,60 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
-        <f ca="1">TODAY()-7</f>
+        <f>DATE(2024,2,5)</f>
+        <v>45327</v>
+      </c>
+      <c r="C2" s="1">
+        <f>B2+1</f>
+        <v>45328</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:O2" si="0">C2+1</f>
+        <v>45329</v>
+      </c>
+      <c r="E2" s="1">
+        <f t="shared" si="0"/>
+        <v>45330</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" si="0"/>
+        <v>45331</v>
+      </c>
+      <c r="G2" s="1">
+        <f t="shared" si="0"/>
+        <v>45332</v>
+      </c>
+      <c r="H2" s="1">
+        <f t="shared" si="0"/>
+        <v>45333</v>
+      </c>
+      <c r="I2" s="1">
+        <f t="shared" si="0"/>
+        <v>45334</v>
+      </c>
+      <c r="J2" s="1">
+        <f t="shared" si="0"/>
+        <v>45335</v>
+      </c>
+      <c r="K2" s="1">
+        <f t="shared" si="0"/>
+        <v>45336</v>
+      </c>
+      <c r="L2" s="1">
+        <f t="shared" si="0"/>
+        <v>45337</v>
+      </c>
+      <c r="M2" s="1">
+        <f t="shared" si="0"/>
+        <v>45338</v>
+      </c>
+      <c r="N2" s="1">
+        <f t="shared" si="0"/>
         <v>45339</v>
       </c>
-      <c r="C2" s="1">
-        <f ca="1">TODAY()-6</f>
+      <c r="O2" s="1">
+        <f t="shared" si="0"/>
         <v>45340</v>
-      </c>
-      <c r="D2" s="1">
-        <f ca="1">TODAY()-5</f>
-        <v>45341</v>
-      </c>
-      <c r="E2" s="1">
-        <f ca="1">TODAY()-4</f>
-        <v>45342</v>
-      </c>
-      <c r="F2" s="1">
-        <f ca="1">TODAY()-3</f>
-        <v>45343</v>
-      </c>
-      <c r="G2" s="1">
-        <f ca="1">TODAY()-2</f>
-        <v>45344</v>
-      </c>
-      <c r="H2" s="1">
-        <f ca="1">TODAY()-1</f>
-        <v>45345</v>
-      </c>
-      <c r="I2" s="1">
-        <f ca="1">TODAY()</f>
-        <v>45346</v>
-      </c>
-      <c r="J2" s="1">
-        <f ca="1">TODAY()+1</f>
-        <v>45347</v>
-      </c>
-      <c r="K2" s="1">
-        <f ca="1">TODAY()+2</f>
-        <v>45348</v>
-      </c>
-      <c r="L2" s="1">
-        <f ca="1">TODAY()+3</f>
-        <v>45349</v>
-      </c>
-      <c r="M2" s="1">
-        <f ca="1">TODAY()+4</f>
-        <v>45350</v>
-      </c>
-      <c r="N2" s="1">
-        <f ca="1">TODAY()+5</f>
-        <v>45351</v>
-      </c>
-      <c r="O2" s="1">
-        <f ca="1">TODAY()+6</f>
-        <v>45352</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -773,7 +772,7 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <v>2</v>
       </c>
       <c r="D5">
@@ -791,7 +790,7 @@
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="16">
         <v>3</v>
       </c>
       <c r="J5" s="10">
@@ -809,7 +808,7 @@
       <c r="N5">
         <v>0</v>
       </c>
-      <c r="O5" s="15">
+      <c r="O5" s="14">
         <v>2</v>
       </c>
     </row>
@@ -822,55 +821,55 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:O7" si="0">B7+C4-C5</f>
+        <f t="shared" ref="C7:O7" si="1">B7+C4-C5</f>
         <v>5</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="O7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -885,60 +884,62 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="16"/>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="15"/>
       <c r="B21" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="B22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="16"/>
       <c r="B23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="14"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="14"/>
       <c r="B27" t="s">
-        <v>39</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -963,33 +964,33 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="16">
+        <v>15</v>
+      </c>
+      <c r="B4" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="16">
+        <v>16</v>
+      </c>
+      <c r="B5" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="9">
         <v>1</v>
@@ -997,20 +998,20 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="17">
+        <v>18</v>
+      </c>
+      <c r="B7" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="11">
         <v>1</v>
@@ -1018,7 +1019,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="10">
         <v>1</v>
@@ -1026,20 +1027,20 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="17">
+        <v>30</v>
+      </c>
+      <c r="B12" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="13">
         <v>1</v>
@@ -1047,7 +1048,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="10">
         <v>1</v>
@@ -1055,36 +1056,36 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="15">
+        <v>22</v>
+      </c>
+      <c r="B19" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="17">
+        <v>23</v>
+      </c>
+      <c r="B20" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="15">
+        <v>24</v>
+      </c>
+      <c r="B21" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <f>B4+B5+B6+B7+B10+B11+B12+B15+B16+B19+B20+B21</f>

</xml_diff>